<commit_message>
sessions on P&L and Mean,Median,Mode completed
</commit_message>
<xml_diff>
--- a/CodeBasics-Excel-GitHub/Mini-Projects/movies_db_cleaned.xlsx
+++ b/CodeBasics-Excel-GitHub/Mini-Projects/movies_db_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shubham-Data-Analytics\Data-Analytics-GitHub\CodeBasics-Excel-GitHub\Mini-Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A095441D-E113-4DDA-BF51-EF4DC1794FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F09301-062B-4CC8-934D-09BE4364859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="actors" sheetId="3" r:id="rId3"/>
     <sheet name="movie_actor" sheetId="4" r:id="rId4"/>
     <sheet name="languages" sheetId="5" r:id="rId5"/>
+    <sheet name="Marvel Financials" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="184">
   <si>
     <t>movie_id</t>
   </si>
@@ -573,13 +575,53 @@
   </si>
   <si>
     <t>% Revenue from Bollywood INR</t>
+  </si>
+  <si>
+    <t>Key Metrics</t>
+  </si>
+  <si>
+    <t>Marvel Consolidated P&amp;L</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Profit/Loss</t>
+  </si>
+  <si>
+    <t>Profit/Loss %</t>
+  </si>
+  <si>
+    <t>Market Share %</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Actuals - Target</t>
+  </si>
+  <si>
+    <t>Actual - Target %</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
@@ -618,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +679,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -647,42 +695,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -765,6 +809,24 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -802,7 +864,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}" name="Movies" displayName="Movies" ref="A1:Q42" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}" name="Movies" displayName="Movies" ref="A1:Q42" headerRowDxfId="17">
   <autoFilter ref="A1:Q42" xr:uid="{6A7FE39D-5614-4A7F-89B7-C167ABC0A251}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{5E453F0D-B27C-433C-BF11-BA3FE1A6822E}" name="movie_id" totalsRowLabel="Total"/>
@@ -812,34 +874,34 @@
     <tableColumn id="5" xr3:uid="{D500D219-E618-40DD-B4AA-E390F996EF1E}" name="imdb_rating"/>
     <tableColumn id="6" xr3:uid="{D06057E5-53B4-474F-BA7C-D7BC731BE502}" name="studio"/>
     <tableColumn id="7" xr3:uid="{70C8CD53-1FFB-4649-B796-093E6560F8C9}" name="language_id"/>
-    <tableColumn id="11" xr3:uid="{6D28D018-B68B-4091-B962-6CF2D3717090}" name="budget" dataDxfId="15">
+    <tableColumn id="11" xr3:uid="{6D28D018-B68B-4091-B962-6CF2D3717090}" name="budget" dataDxfId="16">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[budget]],"Not Available",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0F3F4DA6-833E-4A85-A80F-EC84B27705BC}" name="revenue" dataDxfId="14">
+    <tableColumn id="13" xr3:uid="{0F3F4DA6-833E-4A85-A80F-EC84B27705BC}" name="revenue" dataDxfId="15">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[revenue]],"Not Available",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{191B281A-7053-4160-8EE3-CF6DD1C9435B}" name="unit" dataDxfId="13">
+    <tableColumn id="14" xr3:uid="{191B281A-7053-4160-8EE3-CF6DD1C9435B}" name="unit" dataDxfId="14">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[unit]],"Not Available",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{A197624A-B851-4B51-9B95-7DFC36043837}" name="currency" dataDxfId="12">
+    <tableColumn id="15" xr3:uid="{A197624A-B851-4B51-9B95-7DFC36043837}" name="currency" dataDxfId="13">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{382C3990-7166-463A-A442-412A1810DB4A}" name="budget_mln" dataDxfId="5">
+    <tableColumn id="25" xr3:uid="{382C3990-7166-463A-A442-412A1810DB4A}" name="budget_mln" dataDxfId="12">
       <calculatedColumnFormula>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{E6ED52C2-BDFE-431C-9882-C2EFC4E4B86C}" name="revenue_mln" dataDxfId="4">
+    <tableColumn id="26" xr3:uid="{E6ED52C2-BDFE-431C-9882-C2EFC4E4B86C}" name="revenue_mln" dataDxfId="11">
       <calculatedColumnFormula>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{F7882023-FCA5-486C-AA9D-2F5DDBFE834A}" name="budget_mln_INR" dataDxfId="3">
+    <tableColumn id="27" xr3:uid="{F7882023-FCA5-486C-AA9D-2F5DDBFE834A}" name="budget_mln_INR" dataDxfId="10">
       <calculatedColumnFormula>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{26867AF0-7ABB-440C-9419-EA2BCD8CF886}" name="revenue_mln_INR" dataDxfId="2">
+    <tableColumn id="28" xr3:uid="{26867AF0-7ABB-440C-9419-EA2BCD8CF886}" name="revenue_mln_INR" dataDxfId="9">
       <calculatedColumnFormula>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{56AB7166-A350-461E-BC18-C5188080DF02}" name="budget_mln_USD" dataDxfId="1">
+    <tableColumn id="29" xr3:uid="{56AB7166-A350-461E-BC18-C5188080DF02}" name="budget_mln_USD" dataDxfId="8">
       <calculatedColumnFormula>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{6AA59512-88E5-4086-B22D-01AFCA48CA8E}" name="revenue_mln_USD" dataDxfId="0">
+    <tableColumn id="30" xr3:uid="{6AA59512-88E5-4086-B22D-01AFCA48CA8E}" name="revenue_mln_USD" dataDxfId="7">
       <calculatedColumnFormula>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -848,7 +910,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}" name="Financials" displayName="Financials" ref="A1:E41" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}" name="Financials" displayName="Financials" ref="A1:E41" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:E41" xr:uid="{DCEC907F-917F-4689-8EAB-F7CEF660B9E4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D1A9B0F4-FC15-4DC9-80C7-7EBF56996521}" name="movie_id"/>
@@ -862,7 +924,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49E9627B-7F83-4E00-A9BD-B2B85ADBBA2F}" name="actors" displayName="actors" ref="A1:C68" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49E9627B-7F83-4E00-A9BD-B2B85ADBBA2F}" name="actors" displayName="actors" ref="A1:C68" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:C68" xr:uid="{49E9627B-7F83-4E00-A9BD-B2B85ADBBA2F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{17C41506-36D4-4294-9829-5A0C52DE3455}" name="actor_id"/>
@@ -874,7 +936,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69F3DFB9-F7AC-4F5D-9639-8E5EFD749C75}" name="movieactor" displayName="movieactor" ref="A1:B86" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69F3DFB9-F7AC-4F5D-9639-8E5EFD749C75}" name="movieactor" displayName="movieactor" ref="A1:B86" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:B86" xr:uid="{69F3DFB9-F7AC-4F5D-9639-8E5EFD749C75}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{726AA249-607F-4CEE-9C80-419BD67B7D42}" name="movie_id"/>
@@ -885,7 +947,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C058435-0457-4C21-A779-EC166EB5551A}" name="languages" displayName="languages" ref="A1:B9" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C058435-0457-4C21-A779-EC166EB5551A}" name="languages" displayName="languages" ref="A1:B9" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:B9" xr:uid="{1C058435-0457-4C21-A779-EC166EB5551A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E256DBAD-6FC6-4A32-8A1D-C74A5F599F74}" name="language_id"/>
@@ -1160,11 +1222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q3:Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,27 +1338,27 @@
         <f t="array" ref="K2">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>1000</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>12500</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1000</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>12500</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>12.5</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>156.25</v>
       </c>
@@ -1339,27 +1401,27 @@
         <f t="array" ref="K3">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>200</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>954.8</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>16000</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>76384</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>200</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>954.8</v>
       </c>
@@ -1402,27 +1464,27 @@
         <f t="array" ref="K4">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>165</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>644.79999999999995</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>13200</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>51584</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>165</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>644.79999999999995</v>
       </c>
@@ -1465,27 +1527,27 @@
         <f t="array" ref="K5">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>180</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>854</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>14400</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>68320</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>180</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>854</v>
       </c>
@@ -1528,27 +1590,27 @@
         <f t="array" ref="K6">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>250</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>670</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>20000</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>53600</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>250</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>670</v>
       </c>
@@ -1591,27 +1653,27 @@
         <f t="array" ref="K7">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>Not Available</v>
       </c>
-      <c r="L7" s="4" t="str">
+      <c r="L7" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>Not Available</v>
       </c>
-      <c r="M7" s="4" t="str">
+      <c r="M7" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>Not Available</v>
       </c>
-      <c r="N7" s="4" t="str">
+      <c r="N7" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="O7" s="4" t="str">
+      <c r="O7" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="P7" s="4" t="str">
+      <c r="P7" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="Q7" s="4" t="str">
+      <c r="Q7" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
@@ -1654,27 +1716,27 @@
         <f t="array" ref="K8">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>400</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>2000</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>400</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>2000</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>5</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>25</v>
       </c>
@@ -1717,27 +1779,27 @@
         <f t="array" ref="K9">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>550</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>4000</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>550</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>4000</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>6.875</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>50</v>
       </c>
@@ -1780,27 +1842,27 @@
         <f t="array" ref="K10">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>390</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>1360</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>390</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>1360</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>4.875</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>17</v>
       </c>
@@ -1843,27 +1905,27 @@
         <f t="array" ref="K11">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>1400</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>3500</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1400</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>3500</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>17.5</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>43.75</v>
       </c>
@@ -1906,27 +1968,27 @@
         <f t="array" ref="K12">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>25</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>73.3</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>2000</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>5864</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>25</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>73.3</v>
       </c>
@@ -1969,27 +2031,27 @@
         <f t="array" ref="K13">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>Not Available</v>
       </c>
-      <c r="L13" s="4" t="str">
+      <c r="L13" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>Not Available</v>
       </c>
-      <c r="M13" s="4" t="str">
+      <c r="M13" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>Not Available</v>
       </c>
-      <c r="N13" s="4" t="str">
+      <c r="N13" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="O13" s="4" t="str">
+      <c r="O13" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="P13" s="4" t="str">
+      <c r="P13" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="Q13" s="4" t="str">
+      <c r="Q13" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
@@ -2032,27 +2094,27 @@
         <f t="array" ref="K14">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>165</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>701.8</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>13200</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O14">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>56144</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>165</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>701.8</v>
       </c>
@@ -2095,27 +2157,27 @@
         <f t="array" ref="K15">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>55</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>307.10000000000002</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>4400</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>24568</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>55</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>307.10000000000002</v>
       </c>
@@ -2158,27 +2220,27 @@
         <f t="array" ref="K16">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>103</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>460.5</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>8240</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>36840</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>103</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>460.5</v>
       </c>
@@ -2221,27 +2283,27 @@
         <f t="array" ref="K17">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>200</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>2202</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>16000</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>176160</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>200</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>2202</v>
       </c>
@@ -2284,27 +2346,27 @@
         <f t="array" ref="K18">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>3.18</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>3.3</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>254.4</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>264</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>3.18</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>3.3</v>
       </c>
@@ -2347,27 +2409,27 @@
         <f t="array" ref="K19">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>237</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>2847</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>18960</v>
       </c>
-      <c r="O19" s="4">
+      <c r="O19">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>227760</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>237</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>2847</v>
       </c>
@@ -2410,27 +2472,27 @@
         <f t="array" ref="K20">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>7.2</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>291</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>576</v>
       </c>
-      <c r="O20" s="4">
+      <c r="O20">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>23280</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>7.2</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>291</v>
       </c>
@@ -2473,27 +2535,27 @@
         <f t="array" ref="K21">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>185</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>1006</v>
       </c>
-      <c r="N21" s="4">
+      <c r="N21">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>14800</v>
       </c>
-      <c r="O21" s="4">
+      <c r="O21">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>80480</v>
       </c>
-      <c r="P21" s="4">
+      <c r="P21">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>185</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="Q21">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>1006</v>
       </c>
@@ -2536,27 +2598,27 @@
         <f t="array" ref="K22">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>22</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>322.2</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N22">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1760</v>
       </c>
-      <c r="O22" s="4">
+      <c r="O22">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>25776</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P22">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>22</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="Q22">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>322.2</v>
       </c>
@@ -2599,27 +2661,27 @@
         <f t="array" ref="K23">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>63</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>1046</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>5040</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O23">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>83680</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P23">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>63</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="Q23">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>1046</v>
       </c>
@@ -2662,27 +2724,27 @@
         <f t="array" ref="K24">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>15.5</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>263.10000000000002</v>
       </c>
-      <c r="N24" s="4">
+      <c r="N24">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1240</v>
       </c>
-      <c r="O24" s="4">
+      <c r="O24">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>21048</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>15.5</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q24">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>263.10000000000002</v>
       </c>
@@ -2725,27 +2787,27 @@
         <f t="array" ref="K25">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>400</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>2798</v>
       </c>
-      <c r="N25" s="4">
+      <c r="N25">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>32000</v>
       </c>
-      <c r="O25" s="4">
+      <c r="O25">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>223840</v>
       </c>
-      <c r="P25" s="4">
+      <c r="P25">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>400</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q25">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>2798</v>
       </c>
@@ -2788,27 +2850,27 @@
         <f t="array" ref="K26">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>400</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>2048</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N26">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>32000</v>
       </c>
-      <c r="O26" s="4">
+      <c r="O26">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>163840</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>400</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q26">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>2048</v>
       </c>
@@ -2851,27 +2913,27 @@
         <f t="array" ref="K27">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>70</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>100</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>70</v>
       </c>
-      <c r="O27" s="4">
+      <c r="O27">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>100</v>
       </c>
-      <c r="P27" s="4">
+      <c r="P27">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>0.875</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q27">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>1.25</v>
       </c>
@@ -2914,27 +2976,27 @@
         <f t="array" ref="K28">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>120</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>1350</v>
       </c>
-      <c r="N28" s="4">
+      <c r="N28">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>120</v>
       </c>
-      <c r="O28" s="4">
+      <c r="O28">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>1350</v>
       </c>
-      <c r="P28" s="4">
+      <c r="P28">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>1.5</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="Q28">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>16.875</v>
       </c>
@@ -2977,27 +3039,27 @@
         <f t="array" ref="K29">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>100</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>410</v>
       </c>
-      <c r="N29" s="4">
+      <c r="N29">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>100</v>
       </c>
-      <c r="O29" s="4">
+      <c r="O29">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>410</v>
       </c>
-      <c r="P29" s="4">
+      <c r="P29">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>1.25</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="Q29">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>5.125</v>
       </c>
@@ -3040,27 +3102,27 @@
         <f t="array" ref="K30">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>850</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>8540</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N30">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>850</v>
       </c>
-      <c r="O30" s="4">
+      <c r="O30">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>8540</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>10.625</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q30">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>106.75</v>
       </c>
@@ -3103,27 +3165,27 @@
         <f t="array" ref="K31">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>1000</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>5900</v>
       </c>
-      <c r="N31" s="4">
+      <c r="N31">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1000</v>
       </c>
-      <c r="O31" s="4">
+      <c r="O31">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>5900</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P31">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>12.5</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q31">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>73.75</v>
       </c>
@@ -3166,27 +3228,27 @@
         <f t="array" ref="K32">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>2000</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>3600</v>
       </c>
-      <c r="N32" s="4">
+      <c r="N32">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>2000</v>
       </c>
-      <c r="O32" s="4">
+      <c r="O32">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>3600</v>
       </c>
-      <c r="P32" s="4">
+      <c r="P32">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>25</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="Q32">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>45</v>
       </c>
@@ -3229,27 +3291,27 @@
         <f t="array" ref="K33">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>5500</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>12000</v>
       </c>
-      <c r="N33" s="4">
+      <c r="N33">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>5500</v>
       </c>
-      <c r="O33" s="4">
+      <c r="O33">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>12000</v>
       </c>
-      <c r="P33" s="4">
+      <c r="P33">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>68.75</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="Q33">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>150</v>
       </c>
@@ -3292,27 +3354,27 @@
         <f t="array" ref="K34">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>1800</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>6500</v>
       </c>
-      <c r="N34" s="4">
+      <c r="N34">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1800</v>
       </c>
-      <c r="O34" s="4">
+      <c r="O34">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>6500</v>
       </c>
-      <c r="P34" s="4">
+      <c r="P34">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>22.5</v>
       </c>
-      <c r="Q34" s="4">
+      <c r="Q34">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>81.25</v>
       </c>
@@ -3355,27 +3417,27 @@
         <f t="array" ref="K35">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>250</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>3409</v>
       </c>
-      <c r="N35" s="4">
+      <c r="N35">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>250</v>
       </c>
-      <c r="O35" s="4">
+      <c r="O35">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>3409</v>
       </c>
-      <c r="P35" s="4">
+      <c r="P35">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>3.125</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="Q35">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>42.612499999999997</v>
       </c>
@@ -3418,27 +3480,27 @@
         <f t="array" ref="K36">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>900</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>11690</v>
       </c>
-      <c r="N36" s="4">
+      <c r="N36">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>900</v>
       </c>
-      <c r="O36" s="4">
+      <c r="O36">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>11690</v>
       </c>
-      <c r="P36" s="4">
+      <c r="P36">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>11.25</v>
       </c>
-      <c r="Q36" s="4">
+      <c r="Q36">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>146.125</v>
       </c>
@@ -3481,27 +3543,27 @@
         <f t="array" ref="K37">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>216.7</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>370.6</v>
       </c>
-      <c r="N37" s="4">
+      <c r="N37">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>17336</v>
       </c>
-      <c r="O37" s="4">
+      <c r="O37">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>29648</v>
       </c>
-      <c r="P37" s="4">
+      <c r="P37">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>216.7</v>
       </c>
-      <c r="Q37" s="4">
+      <c r="Q37">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>370.6</v>
       </c>
@@ -3544,27 +3606,27 @@
         <f t="array" ref="K38">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>USD</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>177</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>714.4</v>
       </c>
-      <c r="N38" s="4">
+      <c r="N38">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>14160</v>
       </c>
-      <c r="O38" s="4">
+      <c r="O38">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>57152</v>
       </c>
-      <c r="P38" s="4">
+      <c r="P38">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>177</v>
       </c>
-      <c r="Q38" s="4">
+      <c r="Q38">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>714.4</v>
       </c>
@@ -3607,27 +3669,27 @@
         <f t="array" ref="K39">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>1800</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>3100</v>
       </c>
-      <c r="N39" s="4">
+      <c r="N39">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>1800</v>
       </c>
-      <c r="O39" s="4">
+      <c r="O39">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>3100</v>
       </c>
-      <c r="P39" s="4">
+      <c r="P39">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>22.5</v>
       </c>
-      <c r="Q39" s="4">
+      <c r="Q39">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>38.75</v>
       </c>
@@ -3670,27 +3732,27 @@
         <f t="array" ref="K40">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>INR</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>500</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>950</v>
       </c>
-      <c r="N40" s="4">
+      <c r="N40">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>500</v>
       </c>
-      <c r="O40" s="4">
+      <c r="O40">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>950</v>
       </c>
-      <c r="P40" s="4">
+      <c r="P40">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>6.25</v>
       </c>
-      <c r="Q40" s="4">
+      <c r="Q40">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>11.875</v>
       </c>
@@ -3712,27 +3774,27 @@
         <f t="array" ref="K41">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>Not Available</v>
       </c>
-      <c r="L41" s="4" t="str">
+      <c r="L41" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>Not Available</v>
       </c>
-      <c r="M41" s="4" t="str">
+      <c r="M41" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>Not Available</v>
       </c>
-      <c r="N41" s="4" t="str">
+      <c r="N41" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="O41" s="4" t="str">
+      <c r="O41" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="P41" s="4" t="str">
+      <c r="P41" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="Q41" s="4" t="str">
+      <c r="Q41" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
@@ -3754,59 +3816,59 @@
         <f t="array" ref="K42">_xlfn.XLOOKUP(Movies[[#This Row],[movie_id]:[movie_id]],Financials[[#All],[movie_id]:[movie_id]],Financials[[#All],[currency]],"Not Available",0)</f>
         <v>Not Available</v>
       </c>
-      <c r="L42" s="4" t="str">
+      <c r="L42" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[budget]]*1000,Movies[[#This Row],[budget]])</f>
         <v>Not Available</v>
       </c>
-      <c r="M42" s="4" t="str">
+      <c r="M42" t="str">
         <f>IF(Movies[[#This Row],[unit]]="Billions",Movies[[#This Row],[revenue]]*1000,Movies[[#This Row],[revenue]])</f>
         <v>Not Available</v>
       </c>
-      <c r="N42" s="4" t="str">
+      <c r="N42" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[budget_mln]]*80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="O42" s="4" t="str">
+      <c r="O42" t="str">
         <f>IF(Movies[[#This Row],[currency]]="USD",Movies[[#This Row],[revenue_mln]]*80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="P42" s="4" t="str">
+      <c r="P42" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[budget_mln]]/80,Movies[[#This Row],[budget_mln]])</f>
         <v>Not Available</v>
       </c>
-      <c r="Q42" s="4" t="str">
+      <c r="Q42" t="str">
         <f>IF(Movies[[#This Row],[currency]]="INR",Movies[[#This Row],[revenue_mln]]/80,Movies[[#This Row],[revenue_mln]])</f>
         <v>Not Available</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N44" s="5" t="s">
+      <c r="N44" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="O44" s="5" t="s">
+      <c r="O44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="P44" s="5" t="s">
+      <c r="P44" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="4" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N45" s="6">
+      <c r="N45" s="5">
         <f>SUM(Movies[budget_mln_INR])</f>
         <v>264196.40000000002</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="5">
         <f>SUM(Movies[revenue_mln_INR])</f>
         <v>1567141</v>
       </c>
-      <c r="P45" s="6">
+      <c r="P45" s="5">
         <f>SUM(Movies[budget_mln_USD])</f>
         <v>3302.4549999999999</v>
       </c>
-      <c r="Q45" s="6">
+      <c r="Q45" s="5">
         <f>SUM(Movies[revenue_mln_USD])</f>
         <v>19589.262500000001</v>
       </c>
@@ -3851,7 +3913,7 @@
       <c r="B51" t="s">
         <v>170</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <f>C49/O45</f>
         <v>5.1628411227834639E-2</v>
       </c>
@@ -3859,8 +3921,8 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:B42">
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6769,26 +6831,202 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <MediaLengthInSeconds xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824" xsi:nil="true"/>
-    <SharedWithUsers xmlns="46297aa2-77d1-4586-9726-07d56a535ee7">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C05882-6164-4363-B5FB-B762BBCE24BE}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="8">
+        <f>SUMIF(Movies[studio],"Marvel Studios",Movies[revenue_mln_USD])</f>
+        <v>9054.6</v>
+      </c>
+      <c r="C2" s="8">
+        <v>8000</v>
+      </c>
+      <c r="D2" s="9">
+        <f>B2-C2</f>
+        <v>1054.6000000000004</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2/C2</f>
+        <v>0.13182500000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="8">
+        <f>SUMIF(Movies[studio],"Marvel Studios",Movies[budget_mln_USD])</f>
+        <v>1988.7</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2000</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D6" si="0">B3-C3</f>
+        <v>-11.299999999999955</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E6" si="1">D3/C3</f>
+        <v>-5.6499999999999771E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="8">
+        <f>B2-B3</f>
+        <v>7065.9000000000005</v>
+      </c>
+      <c r="C4" s="8">
+        <v>6000</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>1065.9000000000005</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="1"/>
+        <v>0.17765000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="6">
+        <f>B4/B3</f>
+        <v>3.5530245889274403</v>
+      </c>
+      <c r="C5" s="6">
+        <f>C4/C3</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.55302458892744033</v>
+      </c>
+      <c r="E5" s="6">
+        <f>D5/C5</f>
+        <v>0.1843415296424801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="6">
+        <f>B2/SUMIF(Movies[industry],"Hollywood",Movies[revenue_mln_USD])</f>
+        <v>0.48738554949698293</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>-6.2614450503017116E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>-0.11384445546003111</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>-0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF77FEE3-DBFE-4B13-A28D-0C11164C9839}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="3">
+        <f>AVERAGE(Movies[imdb_rating])</f>
+        <v>7.9473684210526319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3">
+        <f>MEDIAN(Movies[imdb_rating])</f>
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4">
+        <f>MODE(Movies[imdb_rating])</f>
+        <v>8.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100686C0266E115364AA9B96DE5BECF7DB6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c921848065db5a49d1de2391ec81580e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="631564f6-0349-4cc5-b00d-7cf3ba42f824" xmlns:ns3="46297aa2-77d1-4586-9726-07d56a535ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff9dd1b7eff9d7fccc1b7fb333026bb0" ns2:_="" ns3:_="">
     <xsd:import namespace="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
@@ -7017,7 +7255,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -7026,18 +7264,26 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
-    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="46297aa2-77d1-4586-9726-07d56a535ee7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <MediaLengthInSeconds xmlns="631564f6-0349-4cc5-b00d-7cf3ba42f824" xsi:nil="true"/>
+    <SharedWithUsers xmlns="46297aa2-77d1-4586-9726-07d56a535ee7">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02BA008F-2FD2-4901-8027-A024DA31C6C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7056,10 +7302,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46297aa2-77d1-4586-9726-07d56a535ee7"/>
+    <ds:schemaRef ds:uri="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
variance, std dev and correlation completed
</commit_message>
<xml_diff>
--- a/CodeBasics-Excel-GitHub/Mini-Projects/movies_db_cleaned.xlsx
+++ b/CodeBasics-Excel-GitHub/Mini-Projects/movies_db_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shubham-Data-Analytics\Data-Analytics-GitHub\CodeBasics-Excel-GitHub\Mini-Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F09301-062B-4CC8-934D-09BE4364859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EABA104-87BB-41A8-9AF3-739326B0D079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="186">
   <si>
     <t>movie_id</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t>Mode</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
+  </si>
+  <si>
+    <t>Variance</t>
   </si>
 </sst>
 </file>
@@ -6978,10 +6984,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF77FEE3-DBFE-4B13-A28D-0C11164C9839}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7021,12 +7027,39 @@
         <v>8.4</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="3">
+        <f>_xlfn.VAR.P(Movies[imdb_rating])</f>
+        <v>1.3577562326869845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="3">
+        <f>_xlfn.STDEV.P(Movies[imdb_rating])</f>
+        <v>1.1652279745556164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100686C0266E115364AA9B96DE5BECF7DB6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c921848065db5a49d1de2391ec81580e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="631564f6-0349-4cc5-b00d-7cf3ba42f824" xmlns:ns3="46297aa2-77d1-4586-9726-07d56a535ee7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ff9dd1b7eff9d7fccc1b7fb333026bb0" ns2:_="" ns3:_="">
     <xsd:import namespace="631564f6-0349-4cc5-b00d-7cf3ba42f824"/>
@@ -7255,15 +7288,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7284,6 +7308,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02BA008F-2FD2-4901-8027-A024DA31C6C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7302,14 +7334,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C97D6F-A515-40FC-959A-7BC863F10CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EEFF9027-FBEF-4910-8EE6-13D64012C7E9}">
   <ds:schemaRefs>

</xml_diff>